<commit_message>
Zapis wynikow dla danej metody/zakresu/zestawu danych, dodanie zakresow: min-max, whiskers, min-max +- 3 probki
</commit_message>
<xml_diff>
--- a/ICP/avg_metrics_ALL_IT2.xlsx
+++ b/ICP/avg_metrics_ALL_IT2.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Dokumenty\praca inżynierska\ICP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B22CD1B6-73B7-428C-8C8E-C7121F445AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE904A66-8256-418A-9A3B-0550E2ABB625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18648" yWindow="0" windowWidth="4392" windowHeight="12960" xr2:uid="{A60F52B5-176C-4D9B-BDC2-BC896793770A}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{A60F52B5-176C-4D9B-BDC2-BC896793770A}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_metrics_static_neue" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="31">
   <si>
     <t>Class</t>
   </si>
@@ -110,6 +123,9 @@
   </si>
   <si>
     <t>WYNIK</t>
+  </si>
+  <si>
+    <t>dla P3 &lt;10!</t>
   </si>
 </sst>
 </file>
@@ -625,10 +641,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -674,107 +690,7 @@
     <cellStyle name="Uwaga" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Zły" xfId="7" builtinId="27" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1147,27 +1063,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD476FB8-E57B-4A44-9D83-664248C33940}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S26" zoomScale="74" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="74" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="27.33203125" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2"/>
-    <col min="25" max="25" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="2"/>
+    <col min="24" max="24" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1200,47 +1116,44 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1272,54 +1185,51 @@
         <v>238</v>
       </c>
       <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="3" t="str">
-        <f>IF(AND($H3&lt;1.5, $H3&gt;0.8, $G3&lt;5),
+      <c r="L3" s="3" t="str">
+        <f>IF(AND($H3&lt;1.5, $H3&gt;0.8, $G3&lt;4),
    $B3 &amp; " - " &amp; $C3 &amp; " - " &amp; $D3,
    "")</f>
         <v>Class1 - P1 - concave</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="2" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="O3" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="P3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R3" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="R3" s="3">
+        <v>1.3240000000000001</v>
+      </c>
       <c r="S3" s="3">
-        <v>1.3240000000000001</v>
-      </c>
-      <c r="T3" s="3">
         <v>7.0713123976843904E-3</v>
       </c>
-      <c r="U3" s="4">
+      <c r="T3" s="4">
         <v>1.32402525330154</v>
       </c>
+      <c r="U3" s="3">
+        <v>1</v>
+      </c>
       <c r="V3" s="3">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="W3" s="3">
         <v>250</v>
       </c>
-      <c r="X3" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y3" s="3" t="str">
-        <f>IF(AND($V3&lt;1.5, $V3&gt;0.8, $U3&lt;5),
-   $P3 &amp; " - " &amp; $Q3 &amp; " - " &amp; $R3,
+      <c r="X3" s="3" t="str">
+        <f>IF(AND($U3&lt;1.5, $U3&gt;0.8, $T3&lt;4),
+   $O3 &amp; " - " &amp; $P3 &amp; " - " &amp; $Q3,
    "")</f>
         <v>Class1 - P1 - concave</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1351,54 +1261,51 @@
         <v>234</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="3" t="str">
-        <f t="shared" ref="M4:M62" si="0">IF(AND($H4&lt;1.5, $H4&gt;0.8, $G4&lt;5),
+      <c r="L4" s="3" t="str">
+        <f t="shared" ref="L4:L8" si="0">IF(AND($H4&lt;1.5, $H4&gt;0.8, $G4&lt;4),
    $B4 &amp; " - " &amp; $C4 &amp; " - " &amp; $D4,
    "")</f>
         <v/>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="2" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="O4" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="P4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="R4" s="3">
+        <v>3.54</v>
+      </c>
       <c r="S4" s="3">
-        <v>3.54</v>
-      </c>
-      <c r="T4" s="3">
         <v>4.9531873413956998E-2</v>
       </c>
-      <c r="U4" s="4">
+      <c r="T4" s="4">
         <v>3.5403730183374198</v>
       </c>
+      <c r="U4" s="3">
+        <v>1.008</v>
+      </c>
       <c r="V4" s="3">
-        <v>1.008</v>
+        <v>250</v>
       </c>
       <c r="W4" s="3">
         <v>250</v>
       </c>
-      <c r="X4" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y4" s="3" t="str">
-        <f t="shared" ref="Y4:Y62" si="1">IF(AND($V4&lt;1.5, $V4&gt;0.8, $U4&lt;5),
-   $P4 &amp; " - " &amp; $Q4 &amp; " - " &amp; $R4,
+      <c r="X4" s="3" t="str">
+        <f t="shared" ref="X4:X14" si="1">IF(AND($U4&lt;1.5, $U4&gt;0.8, $T4&lt;4),
+   $O4 &amp; " - " &amp; $P4 &amp; " - " &amp; $Q4,
    "")</f>
         <v>Class1 - P1 - curvature</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1430,50 +1337,47 @@
         <v>228</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Class1 - P1 - hilbert</v>
-      </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="3">
+      <c r="R5" s="3">
         <v>3.2</v>
       </c>
+      <c r="S5" s="4">
+        <v>4.3361308473495203E-2</v>
+      </c>
       <c r="T5" s="4">
-        <v>4.3361308473495203E-2</v>
-      </c>
-      <c r="U5" s="4">
         <v>3.2003372128815402</v>
       </c>
+      <c r="U5" s="3">
+        <v>1</v>
+      </c>
       <c r="V5" s="3">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="W5" s="3">
         <v>250</v>
       </c>
-      <c r="X5" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y5" s="3" t="str">
+      <c r="X5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Class1 - P1 - hilbert</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1505,50 +1409,47 @@
         <v>240</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Class1 - P1 - line_distance_10</v>
-      </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="3">
+      <c r="R6" s="3">
         <v>2.532</v>
       </c>
+      <c r="S6" s="4">
+        <v>2.8154209563388499E-2</v>
+      </c>
       <c r="T6" s="4">
-        <v>2.8154209563388499E-2</v>
-      </c>
-      <c r="U6" s="4">
         <v>2.5321780491239898</v>
       </c>
+      <c r="U6" s="3">
+        <v>1</v>
+      </c>
       <c r="V6" s="3">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="W6" s="3">
         <v>250</v>
       </c>
-      <c r="X6" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y6" s="3" t="str">
+      <c r="X6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Class1 - P1 - line_distance_10</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1580,50 +1481,47 @@
         <v>143</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R7" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="R7" s="4">
+        <v>2.92205879137697</v>
+      </c>
       <c r="S7" s="4">
-        <v>2.92205879137697</v>
+        <v>1.25779723344274E-2</v>
       </c>
       <c r="T7" s="4">
-        <v>1.25779723344274E-2</v>
-      </c>
-      <c r="U7" s="4">
         <v>2.9220973667297501</v>
       </c>
+      <c r="U7" s="3">
+        <v>3.4039999999999999</v>
+      </c>
       <c r="V7" s="3">
-        <v>3.4039999999999999</v>
+        <v>250</v>
       </c>
       <c r="W7" s="3">
-        <v>250</v>
-      </c>
-      <c r="X7" s="3">
         <v>132</v>
       </c>
-      <c r="Y7" s="3" t="str">
+      <c r="X7" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1655,50 +1553,47 @@
         <v>246</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Class1 - P1 - wavelet</v>
-      </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="3">
+      <c r="R8" s="3">
         <v>2.6019999999999999</v>
       </c>
+      <c r="S8" s="4">
+        <v>2.9345355210180699E-2</v>
+      </c>
       <c r="T8" s="4">
-        <v>2.9345355210180699E-2</v>
-      </c>
-      <c r="U8" s="4">
         <v>2.6021777856769699</v>
       </c>
+      <c r="U8" s="3">
+        <v>1.204</v>
+      </c>
       <c r="V8" s="3">
-        <v>1.204</v>
+        <v>250</v>
       </c>
       <c r="W8" s="3">
         <v>250</v>
       </c>
-      <c r="X8" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y8" s="3" t="str">
+      <c r="X8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Class1 - P1 - wavelet</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1729,49 +1624,48 @@
       <c r="J9">
         <v>205</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="3" t="str">
+        <f t="shared" ref="L4:L62" si="2">IF(AND($H9&lt;1.5, $H9&gt;0.8, $G9&lt;5),
+   $B9 &amp; " - " &amp; $C9 &amp; " - " &amp; $D9,
+   "")</f>
+        <v/>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q9" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" t="s">
         <v>11</v>
       </c>
-      <c r="S9">
+      <c r="R9">
         <v>5.5614035087719298</v>
       </c>
+      <c r="S9" s="1">
+        <v>1.47964840238279E-2</v>
+      </c>
       <c r="T9" s="1">
-        <v>1.47964840238279E-2</v>
-      </c>
-      <c r="U9" s="1">
         <v>5.5614365793570197</v>
       </c>
+      <c r="U9">
+        <v>0.45600000000000002</v>
+      </c>
       <c r="V9">
-        <v>0.45600000000000002</v>
+        <v>250</v>
       </c>
       <c r="W9">
-        <v>250</v>
-      </c>
-      <c r="X9">
         <v>114</v>
       </c>
-      <c r="Y9" s="3" t="str">
+      <c r="X9" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1802,49 +1696,46 @@
       <c r="J10">
         <v>249</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q10" t="s">
-        <v>17</v>
-      </c>
-      <c r="R10" t="s">
         <v>12</v>
       </c>
-      <c r="S10" s="1">
+      <c r="R10" s="1">
         <v>3.92369477911646</v>
       </c>
-      <c r="T10">
+      <c r="S10">
         <v>2.0205038940615601E-2</v>
       </c>
-      <c r="U10" s="1">
+      <c r="T10" s="1">
         <v>3.9237742747370699</v>
       </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
       <c r="V10">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="W10">
-        <v>250</v>
-      </c>
-      <c r="X10">
         <v>249</v>
       </c>
-      <c r="Y10" s="3" t="str">
+      <c r="X10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Class1 - P2 - curvature</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1875,49 +1766,46 @@
       <c r="J11">
         <v>205</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R11" t="s">
         <v>13</v>
       </c>
-      <c r="S11">
+      <c r="R11">
         <v>5.6875</v>
       </c>
+      <c r="S11" s="1">
+        <v>1.47476507902135E-2</v>
+      </c>
       <c r="T11" s="1">
-        <v>1.47476507902135E-2</v>
-      </c>
-      <c r="U11" s="1">
         <v>5.6875323141290801</v>
       </c>
+      <c r="U11">
+        <v>0.44800000000000001</v>
+      </c>
       <c r="V11">
-        <v>0.44800000000000001</v>
+        <v>250</v>
       </c>
       <c r="W11">
-        <v>250</v>
-      </c>
-      <c r="X11">
         <v>112</v>
       </c>
-      <c r="Y11" s="3" t="str">
+      <c r="X11" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -1948,49 +1836,46 @@
       <c r="J12">
         <v>242</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q12" t="s">
-        <v>17</v>
-      </c>
-      <c r="R12" t="s">
         <v>14</v>
       </c>
+      <c r="R12" s="1">
+        <v>3.9860465116279</v>
+      </c>
       <c r="S12" s="1">
-        <v>3.9860465116279</v>
+        <v>1.8240228292908899E-2</v>
       </c>
       <c r="T12" s="1">
-        <v>1.8240228292908899E-2</v>
-      </c>
-      <c r="U12" s="1">
         <v>3.9861143017259</v>
       </c>
+      <c r="U12">
+        <v>0.86</v>
+      </c>
       <c r="V12">
-        <v>0.86</v>
+        <v>250</v>
       </c>
       <c r="W12">
-        <v>250</v>
-      </c>
-      <c r="X12">
         <v>215</v>
       </c>
-      <c r="Y12" s="3" t="str">
+      <c r="X12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Class1 - P2 - line_distance_10</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -2021,49 +1906,46 @@
       <c r="J13">
         <v>219</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R13" t="s">
         <v>15</v>
       </c>
+      <c r="R13" s="1">
+        <v>7.3756512006512001</v>
+      </c>
       <c r="S13" s="1">
-        <v>7.3756512006512001</v>
+        <v>1.9876408920839899E-2</v>
       </c>
       <c r="T13" s="1">
-        <v>1.9876408920839899E-2</v>
-      </c>
-      <c r="U13" s="1">
         <v>7.37569744238733</v>
       </c>
+      <c r="U13">
+        <v>1.9279999999999999</v>
+      </c>
       <c r="V13">
-        <v>1.9279999999999999</v>
+        <v>250</v>
       </c>
       <c r="W13">
-        <v>250</v>
-      </c>
-      <c r="X13">
         <v>78</v>
       </c>
-      <c r="Y13" s="3" t="str">
+      <c r="X13" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -2094,49 +1976,46 @@
       <c r="J14">
         <v>249</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Q14" t="s">
-        <v>17</v>
-      </c>
-      <c r="R14" t="s">
         <v>16</v>
       </c>
-      <c r="S14" s="1">
+      <c r="R14" s="1">
         <v>4.1342975206611499</v>
       </c>
-      <c r="T14">
+      <c r="S14">
         <v>2.1399083286545099E-2</v>
       </c>
-      <c r="U14" s="1">
+      <c r="T14" s="1">
         <v>4.1343827945906204</v>
       </c>
+      <c r="U14">
+        <v>1.0680000000000001</v>
+      </c>
       <c r="V14">
-        <v>1.0680000000000001</v>
+        <v>250</v>
       </c>
       <c r="W14">
-        <v>250</v>
-      </c>
-      <c r="X14">
         <v>242</v>
       </c>
-      <c r="Y14" s="3" t="str">
+      <c r="X14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Class1 - P2 - wavelet</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -2168,50 +2047,51 @@
         <v>232</v>
       </c>
       <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="3" t="str">
+        <f>IF(AND($H15&lt;1.5, $H15&gt;0.8, $G15&lt;10),
+   $B15 &amp; " - " &amp; $C15 &amp; " - " &amp; $D15,
+   "")</f>
+        <v>Class1 - P3 - concave</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P15" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S15" s="4">
+      <c r="R15" s="4">
         <v>1.77830188679245</v>
       </c>
-      <c r="T15" s="3">
+      <c r="S15" s="3">
         <v>2.7539068056728899E-3</v>
       </c>
-      <c r="U15" s="4">
+      <c r="T15" s="4">
         <v>1.77830583200033</v>
       </c>
+      <c r="U15" s="3">
+        <v>0.84799999999999998</v>
+      </c>
       <c r="V15" s="3">
-        <v>0.84799999999999998</v>
+        <v>250</v>
       </c>
       <c r="W15" s="3">
-        <v>250</v>
-      </c>
-      <c r="X15" s="3">
         <v>212</v>
       </c>
-      <c r="Y15" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X15" s="3" t="str">
+        <f>IF(AND($U15&lt;1.5, $U15&gt;0.8, $T15&lt;5),
+   $O15 &amp; " - " &amp; $P15 &amp; " - " &amp; $Q15,
+   "")</f>
         <v>Class1 - P3 - concave</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2243,46 +2123,47 @@
         <v>250</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="3" t="str">
+        <f t="shared" ref="L16:L20" si="3">IF(AND($H16&lt;1.5, $H16&gt;0.8, $G16&lt;10),
+   $B16 &amp; " - " &amp; $C16 &amp; " - " &amp; $D16,
+   "")</f>
+        <v/>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P16" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S16" s="3">
+      <c r="R16" s="3">
         <v>7.3719999999999999</v>
       </c>
+      <c r="S16" s="4">
+        <v>3.8169060118780199E-2</v>
+      </c>
       <c r="T16" s="4">
-        <v>3.8169060118780199E-2</v>
-      </c>
-      <c r="U16" s="4">
         <v>7.3721287232017998</v>
       </c>
+      <c r="U16" s="3">
+        <v>1.1719999999999999</v>
+      </c>
       <c r="V16" s="3">
-        <v>1.1719999999999999</v>
+        <v>250</v>
       </c>
       <c r="W16" s="3">
         <v>250</v>
       </c>
-      <c r="X16" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y16" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X16" s="3" t="str">
+        <f>IF(AND($U16&lt;1.5, $U16&gt;0.8, $T16&lt;5),
+   $O16 &amp; " - " &amp; $P16 &amp; " - " &amp; $Q16,
+   "")</f>
         <v/>
       </c>
     </row>
@@ -2318,46 +2199,45 @@
         <v>236</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Class1 - P3 - hilbert</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P17" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S17" s="4">
+      <c r="R17" s="4">
         <v>2.6376146788990802</v>
       </c>
-      <c r="T17" s="3">
+      <c r="S17" s="3">
         <v>4.1789015341291503E-3</v>
       </c>
-      <c r="U17" s="4">
+      <c r="T17" s="4">
         <v>2.6376206401214399</v>
       </c>
+      <c r="U17" s="3">
+        <v>0.872</v>
+      </c>
       <c r="V17" s="3">
-        <v>0.872</v>
+        <v>250</v>
       </c>
       <c r="W17" s="3">
-        <v>250</v>
-      </c>
-      <c r="X17" s="3">
         <v>218</v>
       </c>
-      <c r="Y17" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X17" s="3" t="str">
+        <f>IF(AND($U17&lt;1.5, $U17&gt;0.8, $T17&lt;5),
+   $O17 &amp; " - " &amp; $P17 &amp; " - " &amp; $Q17,
+   "")</f>
         <v>Class1 - P3 - hilbert</v>
       </c>
     </row>
@@ -2393,46 +2273,45 @@
         <v>250</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P18" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S18" s="4">
+      <c r="R18" s="4">
         <v>6.8211382113821104</v>
       </c>
-      <c r="T18" s="3">
+      <c r="S18" s="3">
         <v>3.1776657667705099E-2</v>
       </c>
-      <c r="U18" s="4">
+      <c r="T18" s="4">
         <v>6.8212408763070096</v>
       </c>
+      <c r="U18" s="3">
+        <v>0.98399999999999999</v>
+      </c>
       <c r="V18" s="3">
-        <v>0.98399999999999999</v>
+        <v>250</v>
       </c>
       <c r="W18" s="3">
-        <v>250</v>
-      </c>
-      <c r="X18" s="3">
         <v>246</v>
       </c>
-      <c r="Y18" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X18" s="3" t="str">
+        <f>IF(AND($U18&lt;1.5, $U18&gt;0.8, $T18&lt;5),
+   $O18 &amp; " - " &amp; $P18 &amp; " - " &amp; $Q18,
+   "")</f>
         <v/>
       </c>
     </row>
@@ -2468,46 +2347,45 @@
         <v>198</v>
       </c>
       <c r="K19" s="3"/>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P19" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S19" s="4">
+      <c r="R19" s="4">
         <v>2.7339573070607499</v>
       </c>
-      <c r="T19" s="3">
+      <c r="S19" s="3">
         <v>5.0573150509926404E-3</v>
       </c>
-      <c r="U19" s="4">
+      <c r="T19" s="4">
         <v>2.7339657770961798</v>
       </c>
+      <c r="U19" s="3">
+        <v>4.1920000000000002</v>
+      </c>
       <c r="V19" s="3">
-        <v>4.1920000000000002</v>
+        <v>250</v>
       </c>
       <c r="W19" s="3">
-        <v>250</v>
-      </c>
-      <c r="X19" s="3">
         <v>145</v>
       </c>
-      <c r="Y19" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X19" s="3" t="str">
+        <f>IF(AND($U19&lt;1.5, $U19&gt;0.8, $T19&lt;5),
+   $O19 &amp; " - " &amp; $P19 &amp; " - " &amp; $Q19,
+   "")</f>
         <v/>
       </c>
     </row>
@@ -2543,46 +2421,45 @@
         <v>250</v>
       </c>
       <c r="K20" s="3"/>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P20" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R20" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="R20" s="4">
+        <v>7.2604166666666599</v>
+      </c>
       <c r="S20" s="4">
-        <v>7.2604166666666599</v>
+        <v>3.6160572856344698E-2</v>
       </c>
       <c r="T20" s="4">
-        <v>3.6160572856344698E-2</v>
-      </c>
-      <c r="U20" s="4">
         <v>7.2605379110596697</v>
       </c>
+      <c r="U20" s="3">
+        <v>1.3520000000000001</v>
+      </c>
       <c r="V20" s="3">
-        <v>1.3520000000000001</v>
+        <v>250</v>
       </c>
       <c r="W20" s="3">
-        <v>250</v>
-      </c>
-      <c r="X20" s="3">
         <v>248</v>
       </c>
-      <c r="Y20" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X20" s="3" t="str">
+        <f>IF(AND($U20&lt;1.5, $U20&gt;0.8, $T20&lt;5),
+   $O20 &amp; " - " &amp; $P20 &amp; " - " &amp; $Q20,
+   "")</f>
         <v/>
       </c>
     </row>
@@ -2617,45 +2494,44 @@
       <c r="J21">
         <v>224</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" t="s">
         <v>19</v>
       </c>
-      <c r="M21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P21" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q21" t="s">
-        <v>10</v>
-      </c>
-      <c r="R21" t="s">
         <v>11</v>
       </c>
+      <c r="R21" s="1">
+        <v>2.23684210526315</v>
+      </c>
       <c r="S21" s="1">
-        <v>2.23684210526315</v>
+        <v>1.2065438024028499E-2</v>
       </c>
       <c r="T21" s="1">
-        <v>1.2065438024028499E-2</v>
-      </c>
-      <c r="U21" s="1">
         <v>2.2368846705046099</v>
       </c>
+      <c r="U21">
+        <v>0.91200000000000003</v>
+      </c>
       <c r="V21">
-        <v>0.91200000000000003</v>
+        <v>250</v>
       </c>
       <c r="W21">
-        <v>250</v>
-      </c>
-      <c r="X21">
         <v>228</v>
       </c>
-      <c r="Y21" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X21" s="3" t="str">
+        <f>IF(AND($U21&lt;1.5, $U21&gt;0.8, $T21&lt;4),
+   $O21 &amp; " - " &amp; $P21 &amp; " - " &amp; $Q21,
+   "")</f>
         <v>Class2 - P1 - concave</v>
       </c>
     </row>
@@ -2690,46 +2566,45 @@
       <c r="J22">
         <v>238</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P22" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q22" t="s">
-        <v>10</v>
-      </c>
-      <c r="R22" t="s">
         <v>12</v>
       </c>
-      <c r="S22">
+      <c r="R22">
         <v>4.3559999999999999</v>
       </c>
+      <c r="S22" s="1">
+        <v>6.1113337456256502E-2</v>
+      </c>
       <c r="T22" s="1">
-        <v>6.1113337456256502E-2</v>
-      </c>
-      <c r="U22" s="1">
         <v>4.3564983106508102</v>
       </c>
+      <c r="U22">
+        <v>1.048</v>
+      </c>
       <c r="V22">
-        <v>1.048</v>
+        <v>250</v>
       </c>
       <c r="W22">
         <v>250</v>
       </c>
-      <c r="X22">
-        <v>250</v>
-      </c>
-      <c r="Y22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class2 - P1 - curvature</v>
+      <c r="X22" s="3" t="str">
+        <f t="shared" ref="X22:X32" si="4">IF(AND($U22&lt;1.5, $U22&gt;0.8, $T22&lt;4),
+   $O22 &amp; " - " &amp; $P22 &amp; " - " &amp; $Q22,
+   "")</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
@@ -2763,45 +2638,42 @@
       <c r="J23">
         <v>240</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O23" t="s">
         <v>19</v>
       </c>
-      <c r="M23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P23" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q23" t="s">
-        <v>10</v>
-      </c>
-      <c r="R23" t="s">
         <v>13</v>
       </c>
+      <c r="R23">
+        <v>3.3279999999999998</v>
+      </c>
       <c r="S23">
-        <v>3.3279999999999998</v>
-      </c>
-      <c r="T23">
         <v>4.5403848232562299E-2</v>
       </c>
-      <c r="U23" s="1">
+      <c r="T23" s="1">
         <v>3.3283487612372999</v>
       </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
       <c r="V23">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="W23">
         <v>250</v>
       </c>
-      <c r="X23">
-        <v>250</v>
-      </c>
-      <c r="Y23" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X23" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P1 - hilbert</v>
       </c>
     </row>
@@ -2836,45 +2708,42 @@
       <c r="J24">
         <v>240</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O24" t="s">
         <v>19</v>
       </c>
-      <c r="M24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P24" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q24" t="s">
-        <v>10</v>
-      </c>
-      <c r="R24" t="s">
         <v>14</v>
       </c>
-      <c r="S24">
+      <c r="R24">
         <v>3.2759999999999998</v>
       </c>
+      <c r="S24" s="1">
+        <v>4.3592535309452903E-2</v>
+      </c>
       <c r="T24" s="1">
-        <v>4.3592535309452903E-2</v>
-      </c>
-      <c r="U24" s="1">
         <v>3.2763211372187402</v>
       </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
       <c r="V24">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="W24">
         <v>250</v>
       </c>
-      <c r="X24">
-        <v>250</v>
-      </c>
-      <c r="Y24" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X24" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P1 - line_distance_10</v>
       </c>
     </row>
@@ -2909,45 +2778,42 @@
       <c r="J25">
         <v>88</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O25" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q25" t="s">
-        <v>10</v>
-      </c>
-      <c r="R25" t="s">
         <v>15</v>
       </c>
-      <c r="S25" s="1">
+      <c r="R25" s="1">
         <v>5.5565476190476097</v>
       </c>
-      <c r="T25">
+      <c r="S25">
         <v>1.7610134195591501E-2</v>
       </c>
-      <c r="U25" s="1">
+      <c r="T25" s="1">
         <v>5.55659372873163</v>
       </c>
+      <c r="U25">
+        <v>0.66</v>
+      </c>
       <c r="V25">
-        <v>0.66</v>
+        <v>250</v>
       </c>
       <c r="W25">
-        <v>250</v>
-      </c>
-      <c r="X25">
         <v>28</v>
       </c>
-      <c r="Y25" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X25" s="3" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2982,45 +2848,42 @@
       <c r="J26">
         <v>241</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" t="s">
         <v>19</v>
       </c>
-      <c r="M26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P26" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q26" t="s">
-        <v>10</v>
-      </c>
-      <c r="R26" t="s">
         <v>16</v>
       </c>
+      <c r="R26">
+        <v>3.4060000000000001</v>
+      </c>
       <c r="S26">
-        <v>3.4060000000000001</v>
-      </c>
-      <c r="T26">
         <v>4.0752192138632598E-2</v>
       </c>
-      <c r="U26" s="1">
+      <c r="T26" s="1">
         <v>3.40628043578758</v>
       </c>
+      <c r="U26">
+        <v>1.304</v>
+      </c>
       <c r="V26">
-        <v>1.304</v>
+        <v>250</v>
       </c>
       <c r="W26">
         <v>250</v>
       </c>
-      <c r="X26">
-        <v>250</v>
-      </c>
-      <c r="Y26" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X26" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P1 - wavelet</v>
       </c>
     </row>
@@ -3056,46 +2919,43 @@
         <v>243</v>
       </c>
       <c r="K27" s="3"/>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M27" s="3"/>
+      <c r="N27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N27" s="3"/>
-      <c r="O27" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P27" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R27" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="R27" s="3">
+        <v>2.3165137614678901</v>
+      </c>
       <c r="S27" s="3">
-        <v>2.3165137614678901</v>
-      </c>
-      <c r="T27" s="3">
         <v>6.3263057026177001E-3</v>
       </c>
-      <c r="U27" s="4">
+      <c r="T27" s="4">
         <v>2.3165264510291999</v>
       </c>
+      <c r="U27" s="3">
+        <v>0.872</v>
+      </c>
       <c r="V27" s="3">
-        <v>0.872</v>
+        <v>250</v>
       </c>
       <c r="W27" s="3">
-        <v>250</v>
-      </c>
-      <c r="X27" s="3">
         <v>218</v>
       </c>
-      <c r="Y27" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X27" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P2 - concave</v>
       </c>
     </row>
@@ -3131,46 +2991,43 @@
         <v>250</v>
       </c>
       <c r="K28" s="3"/>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M28" s="3"/>
+      <c r="N28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P28" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S28" s="3">
+      <c r="R28" s="3">
         <v>3.8639999999999999</v>
       </c>
+      <c r="S28" s="4">
+        <v>2.0814560469909898E-2</v>
+      </c>
       <c r="T28" s="4">
-        <v>2.0814560469909898E-2</v>
-      </c>
-      <c r="U28" s="4">
         <v>3.8640809521358701</v>
       </c>
+      <c r="U28" s="3">
+        <v>1.044</v>
+      </c>
       <c r="V28" s="3">
-        <v>1.044</v>
+        <v>250</v>
       </c>
       <c r="W28" s="3">
         <v>250</v>
       </c>
-      <c r="X28" s="3">
-        <v>250</v>
-      </c>
-      <c r="Y28" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X28" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P2 - curvature</v>
       </c>
     </row>
@@ -3206,46 +3063,43 @@
         <v>239</v>
       </c>
       <c r="K29" s="3"/>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M29" s="3"/>
+      <c r="N29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P29" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="4">
+      <c r="R29" s="4">
         <v>2.6940639269406299</v>
       </c>
-      <c r="T29" s="3">
+      <c r="S29" s="3">
         <v>7.1273800247580498E-3</v>
       </c>
-      <c r="U29" s="4">
+      <c r="T29" s="4">
         <v>2.6940782666104899</v>
       </c>
+      <c r="U29" s="3">
+        <v>0.876</v>
+      </c>
       <c r="V29" s="3">
-        <v>0.876</v>
+        <v>250</v>
       </c>
       <c r="W29" s="3">
-        <v>250</v>
-      </c>
-      <c r="X29" s="3">
         <v>219</v>
       </c>
-      <c r="Y29" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X29" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P2 - hilbert</v>
       </c>
     </row>
@@ -3281,46 +3135,43 @@
         <v>247</v>
       </c>
       <c r="K30" s="3"/>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M30" s="3"/>
+      <c r="N30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P30" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R30" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="R30" s="4">
+        <v>3.9297520661157002</v>
+      </c>
       <c r="S30" s="4">
-        <v>3.9297520661157002</v>
+        <v>1.96901480622775E-2</v>
       </c>
       <c r="T30" s="4">
-        <v>1.96901480622775E-2</v>
-      </c>
-      <c r="U30" s="4">
         <v>3.92982812928715</v>
       </c>
+      <c r="U30" s="3">
+        <v>0.96799999999999997</v>
+      </c>
       <c r="V30" s="3">
-        <v>0.96799999999999997</v>
+        <v>250</v>
       </c>
       <c r="W30" s="3">
-        <v>250</v>
-      </c>
-      <c r="X30" s="3">
         <v>242</v>
       </c>
-      <c r="Y30" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X30" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Class2 - P2 - line_distance_10</v>
       </c>
     </row>
@@ -3356,46 +3207,43 @@
         <v>245</v>
       </c>
       <c r="K31" s="3"/>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M31" s="3"/>
+      <c r="N31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N31" s="3"/>
-      <c r="O31" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P31" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R31" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="R31" s="4">
+        <v>3.7533068783068702</v>
+      </c>
       <c r="S31" s="4">
-        <v>3.7533068783068702</v>
+        <v>1.2351242852894901E-2</v>
       </c>
       <c r="T31" s="4">
-        <v>1.2351242852894901E-2</v>
-      </c>
-      <c r="U31" s="4">
         <v>3.75333512019226</v>
       </c>
+      <c r="U31" s="3">
+        <v>5.74</v>
+      </c>
       <c r="V31" s="3">
-        <v>5.74</v>
+        <v>250</v>
       </c>
       <c r="W31" s="3">
-        <v>250</v>
-      </c>
-      <c r="X31" s="3">
         <v>180</v>
       </c>
-      <c r="Y31" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X31" s="3" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3431,50 +3279,50 @@
         <v>249</v>
       </c>
       <c r="K32" s="3"/>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="M32" s="3"/>
+      <c r="N32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N32" s="3"/>
-      <c r="O32" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P32" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S32" s="4">
+      <c r="R32" s="4">
         <v>4.1858974358974299</v>
       </c>
-      <c r="T32" s="3">
+      <c r="S32" s="3">
         <v>2.14572334201628E-2</v>
       </c>
-      <c r="U32" s="4">
+      <c r="T32" s="4">
         <v>4.1859796839450203</v>
       </c>
+      <c r="U32" s="3">
+        <v>1.1479999999999999</v>
+      </c>
       <c r="V32" s="3">
-        <v>1.1479999999999999</v>
+        <v>250</v>
       </c>
       <c r="W32" s="3">
-        <v>250</v>
-      </c>
-      <c r="X32" s="3">
         <v>247</v>
       </c>
-      <c r="Y32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class2 - P2 - wavelet</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X32" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Y32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>25</v>
       </c>
@@ -3505,49 +3353,50 @@
       <c r="J33">
         <v>213</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" s="3" t="str">
+        <f>IF(AND($H33&lt;1.5, $H33&gt;0.8, $G33&lt;10),
+   $B33 &amp; " - " &amp; $C33 &amp; " - " &amp; $D33,
+   "")</f>
+        <v/>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O33" t="s">
         <v>19</v>
       </c>
-      <c r="M33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q33" t="s">
-        <v>18</v>
-      </c>
-      <c r="R33" t="s">
         <v>11</v>
       </c>
-      <c r="S33" s="1">
+      <c r="R33" s="1">
         <v>1.49693251533742</v>
       </c>
-      <c r="T33">
+      <c r="S33">
         <v>1.80587226254751E-3</v>
       </c>
-      <c r="U33" s="1">
+      <c r="T33" s="1">
         <v>1.49693397990844</v>
       </c>
+      <c r="U33">
+        <v>0.65200000000000002</v>
+      </c>
       <c r="V33">
-        <v>0.65200000000000002</v>
+        <v>250</v>
       </c>
       <c r="W33">
-        <v>250</v>
-      </c>
-      <c r="X33">
         <v>163</v>
       </c>
-      <c r="Y33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X33" s="3" t="str">
+        <f>IF(AND($U33&lt;1.5, $U33&gt;0.8, $T33&lt;10),
+   $O33 &amp; " - " &amp; $P33 &amp; " - " &amp; $Q33,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -3578,49 +3427,50 @@
       <c r="J34">
         <v>250</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" s="3" t="str">
+        <f t="shared" ref="L34:L38" si="5">IF(AND($H34&lt;1.5, $H34&gt;0.8, $G34&lt;10),
+   $B34 &amp; " - " &amp; $C34 &amp; " - " &amp; $D34,
+   "")</f>
+        <v/>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O34" t="s">
         <v>19</v>
       </c>
-      <c r="M34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q34" t="s">
-        <v>18</v>
-      </c>
-      <c r="R34" t="s">
         <v>12</v>
       </c>
+      <c r="R34">
+        <v>8.57</v>
+      </c>
       <c r="S34">
-        <v>8.57</v>
-      </c>
-      <c r="T34">
         <v>5.80937268955782E-2</v>
       </c>
-      <c r="U34" s="1">
+      <c r="T34" s="1">
         <v>8.5702327007516192</v>
       </c>
+      <c r="U34">
+        <v>1.1120000000000001</v>
+      </c>
       <c r="V34">
-        <v>1.1120000000000001</v>
+        <v>250</v>
       </c>
       <c r="W34">
         <v>250</v>
       </c>
-      <c r="X34">
-        <v>250</v>
-      </c>
-      <c r="Y34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X34" s="3" t="str">
+        <f t="shared" ref="X34:X38" si="6">IF(AND($U34&lt;1.5, $U34&gt;0.8, $T34&lt;10),
+   $O34 &amp; " - " &amp; $P34 &amp; " - " &amp; $Q34,
+   "")</f>
+        <v>Class2 - P3 - curvature</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>25</v>
       </c>
@@ -3651,49 +3501,46 @@
       <c r="J35">
         <v>218</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L35" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O35" t="s">
         <v>19</v>
       </c>
-      <c r="M35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q35" t="s">
-        <v>18</v>
-      </c>
-      <c r="R35" t="s">
         <v>13</v>
       </c>
-      <c r="S35" s="1">
+      <c r="R35" s="1">
         <v>2.6779661016949099</v>
       </c>
+      <c r="S35">
+        <v>4.8518360699111298E-3</v>
+      </c>
       <c r="T35">
-        <v>4.8518360699111298E-3</v>
+        <v>2.6779730895042402</v>
       </c>
       <c r="U35">
-        <v>2.6779730895042402</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="V35">
-        <v>0.70799999999999996</v>
+        <v>250</v>
       </c>
       <c r="W35">
-        <v>250</v>
-      </c>
-      <c r="X35">
         <v>177</v>
       </c>
-      <c r="Y35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X35" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
@@ -3724,49 +3571,46 @@
       <c r="J36">
         <v>250</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L36" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O36" t="s">
         <v>19</v>
       </c>
-      <c r="M36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q36" t="s">
-        <v>18</v>
-      </c>
-      <c r="R36" t="s">
         <v>14</v>
       </c>
-      <c r="S36" s="1">
+      <c r="R36" s="1">
         <v>8.52032520325203</v>
       </c>
-      <c r="T36">
+      <c r="S36">
         <v>5.1179395930269003E-2</v>
       </c>
-      <c r="U36" s="1">
+      <c r="T36" s="1">
         <v>8.5205130039898602</v>
       </c>
+      <c r="U36">
+        <v>0.98399999999999999</v>
+      </c>
       <c r="V36">
-        <v>0.98399999999999999</v>
+        <v>250</v>
       </c>
       <c r="W36">
-        <v>250</v>
-      </c>
-      <c r="X36">
         <v>246</v>
       </c>
-      <c r="Y36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X36" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>Class2 - P3 - line_distance_10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
@@ -3797,49 +3641,46 @@
       <c r="J37">
         <v>222</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O37" t="s">
         <v>19</v>
       </c>
-      <c r="M37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q37" t="s">
-        <v>18</v>
-      </c>
-      <c r="R37" t="s">
         <v>15</v>
       </c>
-      <c r="S37" s="1">
+      <c r="R37" s="1">
         <v>2.3836734693877499</v>
       </c>
-      <c r="T37">
+      <c r="S37">
         <v>4.05900700368181E-3</v>
       </c>
-      <c r="U37" s="1">
+      <c r="T37" s="1">
         <v>2.38367962829629</v>
       </c>
+      <c r="U37">
+        <v>2.7759999999999998</v>
+      </c>
       <c r="V37">
-        <v>2.7759999999999998</v>
+        <v>250</v>
       </c>
       <c r="W37">
-        <v>250</v>
-      </c>
-      <c r="X37">
         <v>98</v>
       </c>
-      <c r="Y37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X37" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>25</v>
       </c>
@@ -3870,49 +3711,46 @@
       <c r="J38">
         <v>250</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O38" t="s">
         <v>19</v>
       </c>
-      <c r="M38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q38" t="s">
-        <v>18</v>
-      </c>
-      <c r="R38" t="s">
         <v>16</v>
       </c>
-      <c r="S38" s="1">
+      <c r="R38" s="1">
         <v>8.7237903225806406</v>
       </c>
-      <c r="T38">
+      <c r="S38">
         <v>5.5150338328984597E-2</v>
       </c>
-      <c r="U38" s="1">
+      <c r="T38" s="1">
         <v>8.7240001953874309</v>
       </c>
+      <c r="U38">
+        <v>1.3320000000000001</v>
+      </c>
       <c r="V38">
-        <v>1.3320000000000001</v>
+        <v>250</v>
       </c>
       <c r="W38">
-        <v>250</v>
-      </c>
-      <c r="X38">
         <v>248</v>
       </c>
-      <c r="Y38" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X38" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>Class2 - P3 - wavelet</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
@@ -3944,50 +3782,51 @@
         <v>42</v>
       </c>
       <c r="K39" s="3"/>
-      <c r="L39" s="3" t="s">
+      <c r="L39" s="3" t="str">
+        <f>IF(AND($H39&lt;1.5, $H39&gt;0.8, $G39&lt;4),
+   $B39 &amp; " - " &amp; $C39 &amp; " - " &amp; $D39,
+   "")</f>
+        <v/>
+      </c>
+      <c r="M39" s="3"/>
+      <c r="N39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N39" s="3"/>
-      <c r="O39" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P39" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S39" s="4">
+      <c r="R39" s="4">
         <v>7.3454545454545404</v>
       </c>
-      <c r="T39" s="3">
+      <c r="S39" s="3">
         <v>8.1885921474161197E-2</v>
       </c>
+      <c r="T39" s="4">
+        <v>7.3460002891081198</v>
+      </c>
       <c r="U39" s="4">
-        <v>7.3460002891081198</v>
-      </c>
-      <c r="V39" s="4">
         <v>0.22088353413654599</v>
       </c>
+      <c r="V39" s="3">
+        <v>250</v>
+      </c>
       <c r="W39" s="3">
-        <v>250</v>
-      </c>
-      <c r="X39" s="3">
         <v>55</v>
       </c>
-      <c r="Y39" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X39" s="3" t="str">
+        <f>IF(AND($U39&lt;1.5, $U39&gt;0.8, $T39&lt;4),
+   $O39 &amp; " - " &amp; $P39 &amp; " - " &amp; $Q39,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
@@ -4019,50 +3858,51 @@
         <v>249</v>
       </c>
       <c r="K40" s="3"/>
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="3" t="str">
+        <f t="shared" ref="L40:L50" si="7">IF(AND($H40&lt;1.5, $H40&gt;0.8, $G40&lt;4),
+   $B40 &amp; " - " &amp; $C40 &amp; " - " &amp; $D40,
+   "")</f>
+        <v>Class3 - P1 - curvature</v>
+      </c>
+      <c r="M40" s="3"/>
+      <c r="N40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M40" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="P40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R40" s="4">
+        <v>3.30443548387096</v>
+      </c>
+      <c r="S40" s="3">
+        <v>5.58122467858609E-2</v>
+      </c>
+      <c r="T40" s="4">
+        <v>3.3049468121282</v>
+      </c>
+      <c r="U40" s="4">
+        <v>1.0522088353413599</v>
+      </c>
+      <c r="V40" s="3">
+        <v>250</v>
+      </c>
+      <c r="W40" s="3">
+        <v>248</v>
+      </c>
+      <c r="X40" s="3" t="str">
+        <f t="shared" ref="X40:X50" si="8">IF(AND($U40&lt;1.5, $U40&gt;0.8, $T40&lt;4),
+   $O40 &amp; " - " &amp; $P40 &amp; " - " &amp; $Q40,
+   "")</f>
         <v>Class3 - P1 - curvature</v>
       </c>
-      <c r="N40" s="3"/>
-      <c r="O40" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S40" s="4">
-        <v>3.30443548387096</v>
-      </c>
-      <c r="T40" s="3">
-        <v>5.58122467858609E-2</v>
-      </c>
-      <c r="U40" s="4">
-        <v>3.3049468121282</v>
-      </c>
-      <c r="V40" s="4">
-        <v>1.0522088353413599</v>
-      </c>
-      <c r="W40" s="3">
-        <v>250</v>
-      </c>
-      <c r="X40" s="3">
-        <v>248</v>
-      </c>
-      <c r="Y40" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P1 - curvature</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>25</v>
       </c>
@@ -4094,50 +3934,47 @@
         <v>117</v>
       </c>
       <c r="K41" s="3"/>
-      <c r="L41" s="3" t="s">
+      <c r="L41" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M41" s="3"/>
+      <c r="N41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N41" s="3"/>
-      <c r="O41" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P41" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S41" s="4">
+      <c r="R41" s="4">
         <v>4.0634920634920597</v>
       </c>
-      <c r="T41" s="3">
+      <c r="S41" s="3">
         <v>5.5846863736920403E-2</v>
       </c>
+      <c r="T41" s="4">
+        <v>4.0638993730750199</v>
+      </c>
       <c r="U41" s="4">
-        <v>4.0638993730750199</v>
-      </c>
-      <c r="V41" s="4">
         <v>0.50602409638554202</v>
       </c>
+      <c r="V41" s="3">
+        <v>250</v>
+      </c>
       <c r="W41" s="3">
-        <v>250</v>
-      </c>
-      <c r="X41" s="3">
         <v>126</v>
       </c>
-      <c r="Y41" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X41" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>25</v>
       </c>
@@ -4169,50 +4006,47 @@
         <v>247</v>
       </c>
       <c r="K42" s="3"/>
-      <c r="L42" s="3" t="s">
+      <c r="L42" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Class3 - P1 - line_distance_10</v>
+      </c>
+      <c r="M42" s="3"/>
+      <c r="N42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M42" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="P42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R42" s="4">
+        <v>2.8346774193548301</v>
+      </c>
+      <c r="S42" s="4">
+        <v>4.8045183778122599E-2</v>
+      </c>
+      <c r="T42" s="4">
+        <v>2.8351143455549499</v>
+      </c>
+      <c r="U42" s="4">
+        <v>0.99598393574297095</v>
+      </c>
+      <c r="V42" s="3">
+        <v>250</v>
+      </c>
+      <c r="W42" s="3">
+        <v>248</v>
+      </c>
+      <c r="X42" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>Class3 - P1 - line_distance_10</v>
       </c>
-      <c r="N42" s="3"/>
-      <c r="O42" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R42" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S42" s="4">
-        <v>2.8346774193548301</v>
-      </c>
-      <c r="T42" s="4">
-        <v>4.8045183778122599E-2</v>
-      </c>
-      <c r="U42" s="4">
-        <v>2.8351143455549499</v>
-      </c>
-      <c r="V42" s="4">
-        <v>0.99598393574297095</v>
-      </c>
-      <c r="W42" s="3">
-        <v>250</v>
-      </c>
-      <c r="X42" s="3">
-        <v>248</v>
-      </c>
-      <c r="Y42" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P1 - line_distance_10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
@@ -4238,50 +4072,47 @@
         <v>0</v>
       </c>
       <c r="K43" s="3"/>
-      <c r="L43" s="3" t="s">
+      <c r="L43" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M43" s="3"/>
+      <c r="N43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N43" s="3"/>
-      <c r="O43" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P43" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R43" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="R43" s="4">
+        <v>25.7222222222222</v>
+      </c>
       <c r="S43" s="4">
-        <v>25.7222222222222</v>
+        <v>0.34601583016095799</v>
       </c>
       <c r="T43" s="4">
-        <v>0.34601583016095799</v>
-      </c>
-      <c r="U43" s="4">
         <v>25.724599627020101</v>
       </c>
+      <c r="U43" s="3">
+        <v>0.32128514056224899</v>
+      </c>
       <c r="V43" s="3">
-        <v>0.32128514056224899</v>
+        <v>250</v>
       </c>
       <c r="W43" s="3">
-        <v>250</v>
-      </c>
-      <c r="X43" s="3">
         <v>9</v>
       </c>
-      <c r="Y43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X43" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
@@ -4313,50 +4144,47 @@
         <v>249</v>
       </c>
       <c r="K44" s="3"/>
-      <c r="L44" s="3" t="s">
+      <c r="L44" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Class3 - P1 - wavelet</v>
+      </c>
+      <c r="M44" s="3"/>
+      <c r="N44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M44" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="P44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R44" s="4">
+        <v>2.4734543010752601</v>
+      </c>
+      <c r="S44" s="4">
+        <v>3.8944075774754797E-2</v>
+      </c>
+      <c r="T44" s="4">
+        <v>2.4737920820713502</v>
+      </c>
+      <c r="U44" s="4">
+        <v>1.31325301204819</v>
+      </c>
+      <c r="V44" s="3">
+        <v>250</v>
+      </c>
+      <c r="W44" s="3">
+        <v>248</v>
+      </c>
+      <c r="X44" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>Class3 - P1 - wavelet</v>
       </c>
-      <c r="N44" s="3"/>
-      <c r="O44" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S44" s="4">
-        <v>2.4734543010752601</v>
-      </c>
-      <c r="T44" s="4">
-        <v>3.8944075774754797E-2</v>
-      </c>
-      <c r="U44" s="4">
-        <v>2.4737920820713502</v>
-      </c>
-      <c r="V44" s="4">
-        <v>1.31325301204819</v>
-      </c>
-      <c r="W44" s="3">
-        <v>250</v>
-      </c>
-      <c r="X44" s="3">
-        <v>248</v>
-      </c>
-      <c r="Y44" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P1 - wavelet</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>25</v>
       </c>
@@ -4387,49 +4215,46 @@
       <c r="J45">
         <v>246</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L45" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O45" t="s">
         <v>20</v>
       </c>
-      <c r="M45" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="P45" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>11</v>
+      </c>
+      <c r="R45" s="1">
+        <v>1.92608695652173</v>
+      </c>
+      <c r="S45">
+        <v>3.43195476553983E-3</v>
+      </c>
+      <c r="T45" s="1">
+        <v>1.92609353088946</v>
+      </c>
+      <c r="U45" s="1">
+        <v>0.92369477911646503</v>
+      </c>
+      <c r="V45">
+        <v>250</v>
+      </c>
+      <c r="W45">
+        <v>230</v>
+      </c>
+      <c r="X45" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>Class3 - P2 - concave</v>
       </c>
-      <c r="O45" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P45" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>17</v>
-      </c>
-      <c r="R45" t="s">
-        <v>11</v>
-      </c>
-      <c r="S45" s="1">
-        <v>1.92608695652173</v>
-      </c>
-      <c r="T45">
-        <v>3.43195476553983E-3</v>
-      </c>
-      <c r="U45" s="1">
-        <v>1.92609353088946</v>
-      </c>
-      <c r="V45" s="1">
-        <v>0.92369477911646503</v>
-      </c>
-      <c r="W45">
-        <v>250</v>
-      </c>
-      <c r="X45">
-        <v>230</v>
-      </c>
-      <c r="Y45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P2 - concave</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>25</v>
       </c>
@@ -4460,49 +4285,46 @@
       <c r="J46">
         <v>247</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L46" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O46" t="s">
         <v>20</v>
       </c>
-      <c r="M46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P46" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q46" t="s">
-        <v>17</v>
-      </c>
-      <c r="R46" t="s">
         <v>12</v>
       </c>
+      <c r="R46">
+        <v>4.06989247311828</v>
+      </c>
       <c r="S46">
-        <v>4.06989247311828</v>
+        <v>1.8625916505898302E-2</v>
       </c>
       <c r="T46">
-        <v>1.8625916505898302E-2</v>
-      </c>
-      <c r="U46">
         <v>4.0699673770017402</v>
       </c>
-      <c r="V46" s="1">
+      <c r="U46" s="1">
         <v>1.0401606425702801</v>
       </c>
+      <c r="V46">
+        <v>250</v>
+      </c>
       <c r="W46">
-        <v>250</v>
-      </c>
-      <c r="X46">
         <v>248</v>
       </c>
-      <c r="Y46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P2 - curvature</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X46" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>25</v>
       </c>
@@ -4533,49 +4355,46 @@
       <c r="J47">
         <v>245</v>
       </c>
-      <c r="L47" t="s">
+      <c r="L47" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O47" t="s">
         <v>20</v>
       </c>
-      <c r="M47" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="P47" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>13</v>
+      </c>
+      <c r="R47" s="1">
+        <v>2.9746835443037898</v>
+      </c>
+      <c r="S47">
+        <v>6.0693961297727701E-3</v>
+      </c>
+      <c r="T47" s="1">
+        <v>2.9747005106178301</v>
+      </c>
+      <c r="U47" s="1">
+        <v>0.95180722891566205</v>
+      </c>
+      <c r="V47">
+        <v>250</v>
+      </c>
+      <c r="W47">
+        <v>237</v>
+      </c>
+      <c r="X47" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>Class3 - P2 - hilbert</v>
       </c>
-      <c r="O47" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P47" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>17</v>
-      </c>
-      <c r="R47" t="s">
-        <v>13</v>
-      </c>
-      <c r="S47" s="1">
-        <v>2.9746835443037898</v>
-      </c>
-      <c r="T47">
-        <v>6.0693961297727701E-3</v>
-      </c>
-      <c r="U47" s="1">
-        <v>2.9747005106178301</v>
-      </c>
-      <c r="V47" s="1">
-        <v>0.95180722891566205</v>
-      </c>
-      <c r="W47">
-        <v>250</v>
-      </c>
-      <c r="X47">
-        <v>237</v>
-      </c>
-      <c r="Y47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P2 - hilbert</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -4606,49 +4425,46 @@
       <c r="J48">
         <v>247</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L48" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O48" t="s">
         <v>20</v>
       </c>
-      <c r="M48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q48" t="s">
-        <v>17</v>
-      </c>
-      <c r="R48" t="s">
         <v>14</v>
       </c>
+      <c r="R48" s="1">
+        <v>4.3830645161290303</v>
+      </c>
       <c r="S48" s="1">
-        <v>4.3830645161290303</v>
-      </c>
-      <c r="T48" s="1">
         <v>1.7153993403232402E-2</v>
       </c>
-      <c r="U48">
+      <c r="T48">
         <v>4.3831320558067501</v>
       </c>
-      <c r="V48" s="1">
+      <c r="U48" s="1">
         <v>0.99598393574297095</v>
       </c>
+      <c r="V48">
+        <v>250</v>
+      </c>
       <c r="W48">
-        <v>250</v>
-      </c>
-      <c r="X48">
         <v>248</v>
       </c>
-      <c r="Y48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Class3 - P2 - line_distance_10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X48" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
@@ -4679,49 +4495,46 @@
       <c r="J49">
         <v>236</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L49" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O49" t="s">
         <v>20</v>
       </c>
-      <c r="M49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P49" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q49" t="s">
-        <v>17</v>
-      </c>
-      <c r="R49" t="s">
         <v>15</v>
       </c>
+      <c r="R49" s="1">
+        <v>3.6796585830566402</v>
+      </c>
       <c r="S49" s="1">
-        <v>3.6796585830566402</v>
+        <v>1.08278021836618E-2</v>
       </c>
       <c r="T49" s="1">
-        <v>1.08278021836618E-2</v>
+        <v>3.6796853143747801</v>
       </c>
       <c r="U49" s="1">
-        <v>3.6796853143747801</v>
-      </c>
-      <c r="V49" s="1">
         <v>6.7429718875502003</v>
       </c>
+      <c r="V49">
+        <v>250</v>
+      </c>
       <c r="W49">
-        <v>250</v>
-      </c>
-      <c r="X49">
         <v>206</v>
       </c>
-      <c r="Y49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X49" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
@@ -4752,49 +4565,46 @@
       <c r="J50">
         <v>248</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L50" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O50" t="s">
         <v>20</v>
       </c>
-      <c r="M50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q50" t="s">
-        <v>17</v>
-      </c>
-      <c r="R50" t="s">
         <v>16</v>
       </c>
+      <c r="R50" s="1">
+        <v>3.6404569892473102</v>
+      </c>
       <c r="S50" s="1">
-        <v>3.6404569892473102</v>
+        <v>1.54973889169589E-2</v>
       </c>
       <c r="T50" s="1">
-        <v>1.54973889169589E-2</v>
+        <v>3.6405213072370501</v>
       </c>
       <c r="U50" s="1">
-        <v>3.6405213072370501</v>
-      </c>
-      <c r="V50" s="1">
         <v>1.1566265060240899</v>
       </c>
+      <c r="V50">
+        <v>250</v>
+      </c>
       <c r="W50">
-        <v>250</v>
-      </c>
-      <c r="X50">
         <v>248</v>
       </c>
-      <c r="Y50" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X50" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>Class3 - P2 - wavelet</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>25</v>
       </c>
@@ -4826,50 +4636,51 @@
         <v>240</v>
       </c>
       <c r="K51" s="3"/>
-      <c r="L51" s="3" t="s">
+      <c r="L51" s="3" t="str">
+        <f>IF(AND($H51&lt;1.5, $H51&gt;0.8, $G51&lt;10),
+   $B51 &amp; " - " &amp; $C51 &amp; " - " &amp; $D51,
+   "")</f>
+        <v/>
+      </c>
+      <c r="M51" s="3"/>
+      <c r="N51" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O51" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N51" s="3"/>
-      <c r="O51" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P51" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S51" s="4">
+      <c r="R51" s="4">
         <v>1.78378378378378</v>
       </c>
-      <c r="T51" s="3">
+      <c r="S51" s="3">
         <v>3.34916842886001E-3</v>
       </c>
+      <c r="T51" s="4">
+        <v>1.7837896946401699</v>
+      </c>
       <c r="U51" s="4">
-        <v>1.7837896946401699</v>
-      </c>
-      <c r="V51" s="4">
         <v>0.44578313253011997</v>
       </c>
+      <c r="V51" s="3">
+        <v>250</v>
+      </c>
       <c r="W51" s="3">
-        <v>250</v>
-      </c>
-      <c r="X51" s="3">
         <v>111</v>
       </c>
-      <c r="Y51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X51" s="3" t="str">
+        <f>IF(AND($U51&lt;1.5, $U51&gt;0.8, $T51&lt;10),
+   $O51 &amp; " - " &amp; $P51 &amp; " - " &amp; $Q51,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
@@ -4901,50 +4712,51 @@
         <v>250</v>
       </c>
       <c r="K52" s="3"/>
-      <c r="L52" s="3" t="s">
+      <c r="L52" s="3" t="str">
+        <f t="shared" ref="L52:L56" si="9">IF(AND($H52&lt;1.5, $H52&gt;0.8, $G52&lt;10),
+   $B52 &amp; " - " &amp; $C52 &amp; " - " &amp; $D52,
+   "")</f>
+        <v/>
+      </c>
+      <c r="M52" s="3"/>
+      <c r="N52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O52" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N52" s="3"/>
-      <c r="O52" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P52" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R52" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="R52" s="4">
+        <v>7.9616935483870899</v>
+      </c>
       <c r="S52" s="4">
-        <v>7.9616935483870899</v>
+        <v>5.5082318082984798E-2</v>
       </c>
       <c r="T52" s="4">
-        <v>5.5082318082984798E-2</v>
+        <v>7.9619192107841004</v>
       </c>
       <c r="U52" s="4">
-        <v>7.9619192107841004</v>
-      </c>
-      <c r="V52" s="4">
         <v>1.0562248995983901</v>
       </c>
+      <c r="V52" s="3">
+        <v>250</v>
+      </c>
       <c r="W52" s="3">
-        <v>250</v>
-      </c>
-      <c r="X52" s="3">
         <v>248</v>
       </c>
-      <c r="Y52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X52" s="3" t="str">
+        <f t="shared" ref="X52:X56" si="10">IF(AND($U52&lt;1.5, $U52&gt;0.8, $T52&lt;10),
+   $O52 &amp; " - " &amp; $P52 &amp; " - " &amp; $Q52,
+   "")</f>
+        <v>Class3 - P3 - curvature</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>25</v>
       </c>
@@ -4976,50 +4788,47 @@
         <v>235</v>
       </c>
       <c r="K53" s="3"/>
-      <c r="L53" s="3" t="s">
+      <c r="L53" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M53" s="3"/>
+      <c r="N53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O53" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N53" s="3"/>
-      <c r="O53" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P53" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R53" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="R53" s="3">
+        <v>2.625</v>
+      </c>
       <c r="S53" s="3">
-        <v>2.625</v>
-      </c>
-      <c r="T53" s="3">
         <v>9.4683533051083003E-3</v>
       </c>
+      <c r="T53" s="4">
+        <v>2.62502889352879</v>
+      </c>
       <c r="U53" s="4">
-        <v>2.62502889352879</v>
-      </c>
-      <c r="V53" s="4">
         <v>0.54618473895582298</v>
       </c>
+      <c r="V53" s="3">
+        <v>250</v>
+      </c>
       <c r="W53" s="3">
-        <v>250</v>
-      </c>
-      <c r="X53" s="3">
         <v>136</v>
       </c>
-      <c r="Y53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X53" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>25</v>
       </c>
@@ -5051,50 +4860,47 @@
         <v>247</v>
       </c>
       <c r="K54" s="3"/>
-      <c r="L54" s="3" t="s">
+      <c r="L54" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M54" s="3"/>
+      <c r="N54" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O54" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N54" s="3"/>
-      <c r="O54" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P54" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R54" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="R54" s="3">
+        <v>7.125</v>
+      </c>
       <c r="S54" s="3">
-        <v>7.125</v>
-      </c>
-      <c r="T54" s="3">
         <v>4.3624375711655797E-2</v>
       </c>
-      <c r="U54" s="4">
+      <c r="T54" s="4">
         <v>7.12516052863631</v>
       </c>
+      <c r="U54" s="3">
+        <v>0.96385542168674698</v>
+      </c>
       <c r="V54" s="3">
-        <v>0.96385542168674698</v>
+        <v>250</v>
       </c>
       <c r="W54" s="3">
-        <v>250</v>
-      </c>
-      <c r="X54" s="3">
         <v>240</v>
       </c>
-      <c r="Y54" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X54" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Class3 - P3 - line_distance_10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>25</v>
       </c>
@@ -5126,50 +4932,47 @@
         <v>249</v>
       </c>
       <c r="K55" s="3"/>
-      <c r="L55" s="3" t="s">
+      <c r="L55" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M55" s="3"/>
+      <c r="N55" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O55" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N55" s="3"/>
-      <c r="O55" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P55" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R55" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S55" s="4">
+      <c r="R55" s="4">
         <v>2.6756187062638599</v>
       </c>
-      <c r="T55" s="3">
+      <c r="S55" s="3">
         <v>5.7714786805052199E-3</v>
       </c>
+      <c r="T55" s="4">
+        <v>2.6756297465918601</v>
+      </c>
       <c r="U55" s="4">
-        <v>2.6756297465918601</v>
-      </c>
-      <c r="V55" s="4">
         <v>2.3574297188754998</v>
       </c>
+      <c r="V55" s="3">
+        <v>250</v>
+      </c>
       <c r="W55" s="3">
-        <v>250</v>
-      </c>
-      <c r="X55" s="3">
         <v>93</v>
       </c>
-      <c r="Y55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X55" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>25</v>
       </c>
@@ -5201,50 +5004,47 @@
         <v>250</v>
       </c>
       <c r="K56" s="3"/>
-      <c r="L56" s="3" t="s">
+      <c r="L56" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M56" s="3"/>
+      <c r="N56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O56" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N56" s="3"/>
-      <c r="O56" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P56" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R56" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S56" s="4">
+      <c r="R56" s="4">
         <v>8.3373819163292797</v>
       </c>
-      <c r="T56" s="3">
+      <c r="S56" s="3">
         <v>5.5989001771584702E-2</v>
       </c>
+      <c r="T56" s="4">
+        <v>8.3376050530303196</v>
+      </c>
       <c r="U56" s="4">
-        <v>8.3376050530303196</v>
-      </c>
-      <c r="V56" s="4">
         <v>1.31325301204819</v>
       </c>
+      <c r="V56" s="3">
+        <v>250</v>
+      </c>
       <c r="W56" s="3">
-        <v>250</v>
-      </c>
-      <c r="X56" s="3">
         <v>247</v>
       </c>
-      <c r="Y56" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X56" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Class3 - P3 - wavelet</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>25</v>
       </c>
@@ -5275,19 +5075,23 @@
       <c r="J57">
         <v>47</v>
       </c>
-      <c r="M57" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="L57" s="3" t="str">
+        <f>IF(AND($H57&lt;1.5, $H57&gt;0.8, $G57&lt;4),
+   $B57 &amp; " - " &amp; $C57 &amp; " - " &amp; $D57,
+   "")</f>
         <v>Class4 - P2 - concave</v>
       </c>
-      <c r="P57" t="s">
+      <c r="O57" t="s">
         <v>21</v>
       </c>
-      <c r="Y57" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X57" s="3" t="str">
+        <f>IF(AND($U57&lt;1.5, $U57&gt;0.8, $T57&lt;5),
+   $O57 &amp; " - " &amp; $P57 &amp; " - " &amp; $Q57,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>25</v>
       </c>
@@ -5318,19 +5122,23 @@
       <c r="J58">
         <v>46</v>
       </c>
-      <c r="M58" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="L58" s="3" t="str">
+        <f t="shared" ref="L58:L62" si="11">IF(AND($H58&lt;1.5, $H58&gt;0.8, $G58&lt;4),
+   $B58 &amp; " - " &amp; $C58 &amp; " - " &amp; $D58,
+   "")</f>
         <v>Class4 - P2 - curvature</v>
       </c>
-      <c r="P58" t="s">
+      <c r="O58" t="s">
         <v>21</v>
       </c>
-      <c r="Y58" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X58" s="3" t="str">
+        <f>IF(AND($U58&lt;1.5, $U58&gt;0.8, $T58&lt;5),
+   $O58 &amp; " - " &amp; $P58 &amp; " - " &amp; $Q58,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>25</v>
       </c>
@@ -5361,19 +5169,21 @@
       <c r="J59">
         <v>48</v>
       </c>
-      <c r="M59" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="L59" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>Class4 - P2 - hilbert</v>
       </c>
-      <c r="P59" t="s">
+      <c r="O59" t="s">
         <v>21</v>
       </c>
-      <c r="Y59" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X59" s="3" t="str">
+        <f>IF(AND($U59&lt;1.5, $U59&gt;0.8, $T59&lt;5),
+   $O59 &amp; " - " &amp; $P59 &amp; " - " &amp; $Q59,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>25</v>
       </c>
@@ -5404,19 +5214,21 @@
       <c r="J60">
         <v>43</v>
       </c>
-      <c r="M60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P60" t="s">
+      <c r="L60" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O60" t="s">
         <v>21</v>
       </c>
-      <c r="Y60" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X60" s="3" t="str">
+        <f>IF(AND($U60&lt;1.5, $U60&gt;0.8, $T60&lt;5),
+   $O60 &amp; " - " &amp; $P60 &amp; " - " &amp; $Q60,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>25</v>
       </c>
@@ -5447,19 +5259,21 @@
       <c r="J61">
         <v>48</v>
       </c>
-      <c r="M61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P61" t="s">
+      <c r="L61" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O61" t="s">
         <v>21</v>
       </c>
-      <c r="Y61" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X61" s="3" t="str">
+        <f>IF(AND($U61&lt;1.5, $U61&gt;0.8, $T61&lt;5),
+   $O61 &amp; " - " &amp; $P61 &amp; " - " &amp; $Q61,
+   "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -5490,42 +5304,38 @@
       <c r="J62">
         <v>46</v>
       </c>
-      <c r="M62" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="L62" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>Class4 - P2 - wavelet</v>
       </c>
-      <c r="P62" t="s">
+      <c r="O62" t="s">
         <v>21</v>
       </c>
-      <c r="Y62" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="X62" s="3" t="str">
+        <f>IF(AND($U62&lt;1.5, $U62&gt;0.8, $T62&lt;5),
+   $O62 &amp; " - " &amp; $P62 &amp; " - " &amp; $Q62,
+   "")</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576 U1:U1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>0.9</formula>
+      <formula>1.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
       <formula>0.6</formula>
       <formula>1.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
       <formula>"0.8"</formula>
       <formula>45689</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
-      <formula>0.6</formula>
-      <formula>1.4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576 V1:V1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
-      <formula>0.9</formula>
-      <formula>1.1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1048576 G1:G1048576">
+  <conditionalFormatting sqref="T1:T1048576 G1:G1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5537,6 +5347,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U1048576">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>0.6</formula>
+      <formula>1.4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>